<commit_message>
Update export tempates to 2022.06.21
</commit_message>
<xml_diff>
--- a/src/server/data/treasury/subRecipientBulkUpload.xlsx
+++ b/src/server/data/treasury/subRecipientBulkUpload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\OneDrive - ICF\Documents\BulkUploadTemplates\4.5 Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/42853_icf_com/Documents/Bulk Upload/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D41E6C-A8AF-4DBE-9C08-D520B14379A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CDDF2DDD-2ACC-4F7F-B918-E1A7C7EF68C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D629BCD-332D-4306-A0BB-DFCCF03D903D}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Recipient-Clean-Data (1)" sheetId="1" r:id="rId1"/>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Entity Type</t>
+  </si>
+  <si>
+    <t>Version: 2022.03.28</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions to Reporter:
@@ -310,9 +313,6 @@
 -Subrecipient;  
 -Contractor;
 -Beneficiary;</t>
-  </si>
-  <si>
-    <t>Version: 2022.04.07</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7:AA7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -685,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -747,7 +749,7 @@
     </row>
     <row r="3" spans="1:27" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -790,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
@@ -903,43 +905,43 @@
         <v>49</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="18" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -947,10 +949,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>26</v>
@@ -992,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>38</v>
@@ -1030,16 +1032,16 @@
         <v>51</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>53</v>
@@ -1069,43 +1071,43 @@
         <v>61</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="W7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="X7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="Y7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Z7" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="AA7" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Treasury exports v2022.06.21 (#397)
* Update export tempates to 2022.06.21

* Update all template references in code

* Update: generateProjectBaseline

* Update: generateProject18

* Update: generateProject19

* Update: generateProject31

* Update: generateProject32

* Update: generateProject236

* Update: generateProject2128

* Update: generateProject4142

* Update: generateProject51518

* Implement: generateProject111210

* Implement: generateProject211214

* Implement: generateProject215218

* Implement: generateProject224227

* Update: generateProject519521
</commit_message>
<xml_diff>
--- a/src/server/data/treasury/subRecipientBulkUpload.xlsx
+++ b/src/server/data/treasury/subRecipientBulkUpload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\OneDrive - ICF\Documents\BulkUploadTemplates\4.5 Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline-my.sharepoint.com/personal/42853_icf_com/Documents/Bulk Upload/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D41E6C-A8AF-4DBE-9C08-D520B14379A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CDDF2DDD-2ACC-4F7F-B918-E1A7C7EF68C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D629BCD-332D-4306-A0BB-DFCCF03D903D}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Recipient-Clean-Data (1)" sheetId="1" r:id="rId1"/>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Entity Type</t>
+  </si>
+  <si>
+    <t>Version: 2022.03.28</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions to Reporter:
@@ -310,9 +313,6 @@
 -Subrecipient;  
 -Contractor;
 -Beneficiary;</t>
-  </si>
-  <si>
-    <t>Version: 2022.04.07</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7:AA7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -685,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -747,7 +749,7 @@
     </row>
     <row r="3" spans="1:27" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -790,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>4</v>
@@ -903,43 +905,43 @@
         <v>49</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:27" s="18" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -947,10 +949,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>26</v>
@@ -992,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>38</v>
@@ -1030,16 +1032,16 @@
         <v>51</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>53</v>
@@ -1069,43 +1071,43 @@
         <v>61</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="W7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="X7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="Y7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Z7" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="AA7" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>